<commit_message>
did some control stufferino xd
</commit_message>
<xml_diff>
--- a/src/documents/Orwb_Gantt.xlsx
+++ b/src/documents/Orwb_Gantt.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IMS\Orwb\src\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100010_{C71AA358-51FC-4649-95DD-7C3A2A9391A9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplaner" sheetId="1" r:id="rId1"/>
+    <sheet name="Arbeitsjournal" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Projektplaner!$3:$4</definedName>
@@ -27,7 +27,7 @@
     <definedName name="ZeitraumInPlan">Projektplaner!A$4=MEDIAN(Projektplaner!A$4,Projektplaner!$D1,Projektplaner!$D1+Projektplaner!$E1-1)</definedName>
     <definedName name="ZeitraumInTatsächlich">Projektplaner!A$4=MEDIAN(Projektplaner!A$4,Projektplaner!$F1,Projektplaner!$F1+Projektplaner!$G1-1)</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>Wählen Sie rechts einen Zeitraum zum Hervorheben aus.  Es folgt eine Legende, die das Diagramm beschreibt.</t>
   </si>
@@ -239,15 +239,63 @@
   <si>
     <t>Ferien</t>
   </si>
+  <si>
+    <t>Tätigkeit</t>
+  </si>
+  <si>
+    <t>Bemerkungen</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Ausarbeitung Konzept</t>
+  </si>
+  <si>
+    <t>Zeitaufwand in h</t>
+  </si>
+  <si>
+    <t>Website Framework</t>
+  </si>
+  <si>
+    <t>Installieren aller benötigen libraries</t>
+  </si>
+  <si>
+    <t>17.013.2019</t>
+  </si>
+  <si>
+    <t>14.01.2019</t>
+  </si>
+  <si>
+    <t>19.01.2019</t>
+  </si>
+  <si>
+    <t>20.01.2019</t>
+  </si>
+  <si>
+    <t>Einarbitung P5</t>
+  </si>
+  <si>
+    <t>Einarbeitung OO Js</t>
+  </si>
+  <si>
+    <t>21.01.2019</t>
+  </si>
+  <si>
+    <t>Anpassug Website</t>
+  </si>
+  <si>
+    <t>Einarbeitung P5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-407]d\.\ mmm\.;@"/>
+    <numFmt numFmtId="164" formatCode="[$-407]d\.\ mmm\.;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -346,6 +394,12 @@
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -557,7 +611,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,6 +654,42 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="14" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="8" xfId="3" applyBorder="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -633,63 +723,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="8" xfId="3" applyBorder="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="% abgeschlossen" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Aktivität" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Bezeichnung" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="% abgeschlossen" xfId="16"/>
+    <cellStyle name="Aktivität" xfId="2"/>
+    <cellStyle name="Bezeichnung" xfId="5"/>
     <cellStyle name="Erklärender Text" xfId="12" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Legende &quot;Tatsächlich&quot;" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Legende zu &quot;% abgeschlossen (hinter dem Plan)&quot;" xfId="18" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Legende zu &quot;tatsächlich (hinter dem Plan)&quot;" xfId="17" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Planlegende" xfId="14" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Projektüberschriften" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Prozent abgeschlossen" xfId="6" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Legende &quot;Tatsächlich&quot;" xfId="15"/>
+    <cellStyle name="Legende zu &quot;% abgeschlossen (hinter dem Plan)&quot;" xfId="18"/>
+    <cellStyle name="Legende zu &quot;tatsächlich (hinter dem Plan)&quot;" xfId="17"/>
+    <cellStyle name="Planlegende" xfId="14"/>
+    <cellStyle name="Projektüberschriften" xfId="4"/>
+    <cellStyle name="Prozent abgeschlossen" xfId="6"/>
     <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Steuerelement zum Hervorheben von Zeiträumen" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Steuerelement zum Hervorheben von Zeiträumen" xfId="7"/>
     <cellStyle name="Überschrift" xfId="8" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Überschrift 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Überschrift 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Überschriften für Zeiträume" xfId="3" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Zeitraumwert" xfId="13" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Überschriften für Zeiträume" xfId="3"/>
+    <cellStyle name="Zeitraumwert" xfId="13"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1073,14 +1136,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:BJ30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1147,10 +1210,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:62" ht="60" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="36"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
@@ -1158,14 +1221,14 @@
       <c r="H1" s="11"/>
     </row>
     <row r="2" spans="2:62" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="5" t="s">
         <v>31</v>
       </c>
@@ -1173,249 +1236,249 @@
         <v>4</v>
       </c>
       <c r="K2" s="13"/>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="23" t="s">
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="14" t="s">
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="29"/>
-      <c r="AB2" s="24" t="s">
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="14" t="s">
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="36"/>
+      <c r="AI2" s="17"/>
+      <c r="AJ2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="AK2" s="14"/>
-      <c r="AL2" s="14"/>
-      <c r="AM2" s="14"/>
-      <c r="AN2" s="14"/>
-      <c r="AO2" s="14"/>
-      <c r="AP2" s="14"/>
-      <c r="AQ2" s="14"/>
-      <c r="AR2" s="26" t="s">
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
+      <c r="AN2" s="26"/>
+      <c r="AO2" s="26"/>
+      <c r="AP2" s="26"/>
+      <c r="AQ2" s="26"/>
+      <c r="AR2" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AT2" s="34" t="s">
+      <c r="AT2" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:62" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="14">
         <v>43472</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="14">
         <v>43473</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="14">
         <v>43474</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3" s="14">
         <v>43475</v>
       </c>
-      <c r="M3" s="25">
+      <c r="M3" s="14">
         <v>43476</v>
       </c>
-      <c r="N3" s="25">
+      <c r="N3" s="14">
         <v>43477</v>
       </c>
-      <c r="O3" s="25">
+      <c r="O3" s="14">
         <v>43478</v>
       </c>
-      <c r="P3" s="25">
+      <c r="P3" s="14">
         <v>43479</v>
       </c>
-      <c r="Q3" s="25">
+      <c r="Q3" s="14">
         <v>43480</v>
       </c>
-      <c r="R3" s="25">
+      <c r="R3" s="14">
         <v>43481</v>
       </c>
-      <c r="S3" s="25">
+      <c r="S3" s="14">
         <v>43482</v>
       </c>
-      <c r="T3" s="25">
+      <c r="T3" s="14">
         <v>43483</v>
       </c>
-      <c r="U3" s="25">
+      <c r="U3" s="14">
         <v>43484</v>
       </c>
-      <c r="V3" s="25">
+      <c r="V3" s="14">
         <v>43485</v>
       </c>
-      <c r="W3" s="25">
+      <c r="W3" s="14">
         <v>43486</v>
       </c>
-      <c r="X3" s="25">
+      <c r="X3" s="14">
         <v>43487</v>
       </c>
-      <c r="Y3" s="25">
+      <c r="Y3" s="14">
         <v>43488</v>
       </c>
-      <c r="Z3" s="25">
+      <c r="Z3" s="14">
         <v>43489</v>
       </c>
-      <c r="AA3" s="25">
+      <c r="AA3" s="14">
         <v>43490</v>
       </c>
-      <c r="AB3" s="27">
+      <c r="AB3" s="16">
         <v>43491</v>
       </c>
-      <c r="AC3" s="27">
+      <c r="AC3" s="16">
         <v>43492</v>
       </c>
-      <c r="AD3" s="27">
+      <c r="AD3" s="16">
         <v>43493</v>
       </c>
-      <c r="AE3" s="27">
+      <c r="AE3" s="16">
         <v>43494</v>
       </c>
-      <c r="AF3" s="27">
+      <c r="AF3" s="16">
         <v>43495</v>
       </c>
-      <c r="AG3" s="27">
+      <c r="AG3" s="16">
         <v>43496</v>
       </c>
-      <c r="AH3" s="27">
+      <c r="AH3" s="16">
         <v>43497</v>
       </c>
-      <c r="AI3" s="27">
+      <c r="AI3" s="16">
         <v>43498</v>
       </c>
-      <c r="AJ3" s="27">
+      <c r="AJ3" s="16">
         <v>43499</v>
       </c>
-      <c r="AK3" s="25">
+      <c r="AK3" s="14">
         <v>43500</v>
       </c>
-      <c r="AL3" s="25">
+      <c r="AL3" s="14">
         <v>43501</v>
       </c>
-      <c r="AM3" s="25">
+      <c r="AM3" s="14">
         <v>43502</v>
       </c>
-      <c r="AN3" s="25">
+      <c r="AN3" s="14">
         <v>43503</v>
       </c>
-      <c r="AO3" s="25">
+      <c r="AO3" s="14">
         <v>43504</v>
       </c>
-      <c r="AP3" s="25">
+      <c r="AP3" s="14">
         <v>43505</v>
       </c>
-      <c r="AQ3" s="25">
+      <c r="AQ3" s="14">
         <v>43506</v>
       </c>
-      <c r="AR3" s="25">
+      <c r="AR3" s="14">
         <v>43507</v>
       </c>
-      <c r="AS3" s="25">
+      <c r="AS3" s="14">
         <v>43508</v>
       </c>
-      <c r="AT3" s="25">
+      <c r="AT3" s="14">
         <v>43509</v>
       </c>
-      <c r="AU3" s="25">
+      <c r="AU3" s="14">
         <v>43510</v>
       </c>
-      <c r="AV3" s="25">
+      <c r="AV3" s="14">
         <v>43511</v>
       </c>
-      <c r="AW3" s="25">
+      <c r="AW3" s="14">
         <v>43512</v>
       </c>
-      <c r="AX3" s="25">
+      <c r="AX3" s="14">
         <v>43513</v>
       </c>
-      <c r="AY3" s="25">
+      <c r="AY3" s="14">
         <v>43514</v>
       </c>
-      <c r="AZ3" s="25">
+      <c r="AZ3" s="14">
         <v>43515</v>
       </c>
-      <c r="BA3" s="25">
+      <c r="BA3" s="14">
         <v>43516</v>
       </c>
-      <c r="BB3" s="25">
+      <c r="BB3" s="14">
         <v>43517</v>
       </c>
-      <c r="BC3" s="25">
+      <c r="BC3" s="14">
         <v>43518</v>
       </c>
-      <c r="BD3" s="25">
+      <c r="BD3" s="14">
         <v>43519</v>
       </c>
-      <c r="BE3" s="25">
+      <c r="BE3" s="14">
         <v>43520</v>
       </c>
-      <c r="BF3" s="25">
+      <c r="BF3" s="14">
         <v>43521</v>
       </c>
-      <c r="BG3" s="25">
+      <c r="BG3" s="14">
         <v>43522</v>
       </c>
-      <c r="BH3" s="25">
+      <c r="BH3" s="14">
         <v>43523</v>
       </c>
-      <c r="BI3" s="25">
+      <c r="BI3" s="14">
         <v>43524</v>
       </c>
-      <c r="BJ3" s="35">
+      <c r="BJ3" s="24">
         <v>43525</v>
       </c>
     </row>
     <row r="4" spans="2:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="32">
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="21">
         <v>1</v>
       </c>
       <c r="J4" s="3">
@@ -1597,7 +1660,7 @@
       <c r="H5" s="8">
         <v>0.5</v>
       </c>
-      <c r="I5" s="33"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="6" t="s">
@@ -1618,7 +1681,7 @@
       <c r="H6" s="8">
         <v>1</v>
       </c>
-      <c r="I6" s="33"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="6" t="s">
@@ -1639,7 +1702,7 @@
       <c r="H7" s="8">
         <v>0.35</v>
       </c>
-      <c r="I7" s="33"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="6" t="s">
@@ -1660,7 +1723,7 @@
       <c r="H8" s="8">
         <v>0.1</v>
       </c>
-      <c r="I8" s="33"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="6" t="s">
@@ -1681,7 +1744,7 @@
       <c r="H9" s="8">
         <v>0.85</v>
       </c>
-      <c r="I9" s="33"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="6" t="s">
@@ -1702,7 +1765,7 @@
       <c r="H10" s="8">
         <v>0.85</v>
       </c>
-      <c r="I10" s="33"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="6" t="s">
@@ -1723,7 +1786,7 @@
       <c r="H11" s="8">
         <v>0.5</v>
       </c>
-      <c r="I11" s="33"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="6" t="s">
@@ -1744,7 +1807,7 @@
       <c r="H12" s="8">
         <v>0.6</v>
       </c>
-      <c r="I12" s="33"/>
+      <c r="I12" s="22"/>
     </row>
     <row r="13" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="6" t="s">
@@ -1765,7 +1828,7 @@
       <c r="H13" s="8">
         <v>0.75</v>
       </c>
-      <c r="I13" s="33"/>
+      <c r="I13" s="22"/>
     </row>
     <row r="14" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="6" t="s">
@@ -1786,7 +1849,7 @@
       <c r="H14" s="8">
         <v>1</v>
       </c>
-      <c r="I14" s="33"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="6" t="s">
@@ -1807,7 +1870,7 @@
       <c r="H15" s="8">
         <v>0.6</v>
       </c>
-      <c r="I15" s="33"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="6" t="s">
@@ -1828,7 +1891,7 @@
       <c r="H16" s="8">
         <v>0</v>
       </c>
-      <c r="I16" s="33"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="6" t="s">
@@ -1849,7 +1912,7 @@
       <c r="H17" s="8">
         <v>0.5</v>
       </c>
-      <c r="I17" s="33"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="6" t="s">
@@ -1870,7 +1933,7 @@
       <c r="H18" s="8">
         <v>0</v>
       </c>
-      <c r="I18" s="33"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="6" t="s">
@@ -1891,7 +1954,7 @@
       <c r="H19" s="8">
         <v>0.01</v>
       </c>
-      <c r="I19" s="33"/>
+      <c r="I19" s="22"/>
     </row>
     <row r="20" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="6" t="s">
@@ -1912,7 +1975,7 @@
       <c r="H20" s="8">
         <v>0.8</v>
       </c>
-      <c r="I20" s="33"/>
+      <c r="I20" s="22"/>
     </row>
     <row r="21" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="6" t="s">
@@ -1933,7 +1996,7 @@
       <c r="H21" s="8">
         <v>0</v>
       </c>
-      <c r="I21" s="33"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="22" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="6" t="s">
@@ -1954,7 +2017,7 @@
       <c r="H22" s="8">
         <v>0</v>
       </c>
-      <c r="I22" s="33"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="6" t="s">
@@ -1975,7 +2038,7 @@
       <c r="H23" s="8">
         <v>0</v>
       </c>
-      <c r="I23" s="33"/>
+      <c r="I23" s="22"/>
     </row>
     <row r="24" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="6" t="s">
@@ -1996,7 +2059,7 @@
       <c r="H24" s="8">
         <v>0</v>
       </c>
-      <c r="I24" s="33"/>
+      <c r="I24" s="22"/>
     </row>
     <row r="25" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="6" t="s">
@@ -2017,7 +2080,7 @@
       <c r="H25" s="8">
         <v>0.44</v>
       </c>
-      <c r="I25" s="33"/>
+      <c r="I25" s="22"/>
     </row>
     <row r="26" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="6" t="s">
@@ -2038,7 +2101,7 @@
       <c r="H26" s="8">
         <v>0</v>
       </c>
-      <c r="I26" s="33"/>
+      <c r="I26" s="22"/>
     </row>
     <row r="27" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="6" t="s">
@@ -2059,7 +2122,7 @@
       <c r="H27" s="8">
         <v>0.12</v>
       </c>
-      <c r="I27" s="33"/>
+      <c r="I27" s="22"/>
     </row>
     <row r="28" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="6" t="s">
@@ -2080,7 +2143,7 @@
       <c r="H28" s="8">
         <v>0.05</v>
       </c>
-      <c r="I28" s="33"/>
+      <c r="I28" s="22"/>
     </row>
     <row r="29" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="6" t="s">
@@ -2101,7 +2164,7 @@
       <c r="H29" s="8">
         <v>0</v>
       </c>
-      <c r="I29" s="33"/>
+      <c r="I29" s="22"/>
     </row>
     <row r="30" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="6" t="s">
@@ -2122,7 +2185,7 @@
       <c r="H30" s="8">
         <v>0.5</v>
       </c>
-      <c r="I30" s="33"/>
+      <c r="I30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2178,23 +2241,23 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="28" yWindow="315" count="15">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Der Projektplaner verwendet Zeiträume als Intervalle. Start=1 bedeutet Zeitraum 1, und Dauer=5 bedeutet, dass das Projekt 5 Zeiträume ab dem Startzeitraum umfasst. Geben Sie von B5 an Daten ein, um das Diagramm zu aktualisieren" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Geben Sie einen Wert von 1 bis 60 ein, oder wählen Sie in der Liste einen Zeitraum aus – drücken Sie ABBRECHEN, ALT+NACH-UNTEN und dann die EINGABETASTE, um einen Wert auszuwählen" prompt="Geben Sie einen Zeitraum im Bereich von 1 bis 60 ein, oder wählen Sie einen Zeitraum in der Liste aus. Drücken Sie ALT+NACH-UNTEN, um in der Liste zu navigieren, und dann EINGABE, um einen Wert auszuwählen." sqref="I2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Der Projektplaner verwendet Zeiträume als Intervalle. Start=1 bedeutet Zeitraum 1, und Dauer=5 bedeutet, dass das Projekt 5 Zeiträume ab dem Startzeitraum umfasst. Geben Sie von B5 an Daten ein, um das Diagramm zu aktualisieren" sqref="A1"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Geben Sie einen Wert von 1 bis 60 ein, oder wählen Sie in der Liste einen Zeitraum aus – drücken Sie ABBRECHEN, ALT+NACH-UNTEN und dann die EINGABETASTE, um einen Wert auszuwählen" prompt="Geben Sie einen Zeitraum im Bereich von 1 bis 60 ein, oder wählen Sie einen Zeitraum in der Liste aus. Drücken Sie ALT+NACH-UNTEN, um in der Liste zu navigieren, und dann EINGABE, um einen Wert auszuwählen." sqref="I2">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die Dauer des Plans an" sqref="K2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die tatsächliche Dauer an" sqref="Q2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt den Prozentsatz der Fertigstellung des Projekts an" sqref="V2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die tatsächliche Dauer über den Plan hinaus an" sqref="AA2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt den Prozentsatz der Fertigstellung des Projekts über den Plan hinaus an" sqref="AI2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den Startzeitraum des Plans in Spalte C ein, beginnend mit Zelle C5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie die Dauer in Zeiträumen für den Plan in Spalte D ein, beginnend mit Zelle D5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den tatsächlichen Startzeitraum des Plans in Spalte E ein, beginnend mit Zelle E5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie die tatsächliche Dauer in Zeiträumen für den Plan in Spalte F ein, beginnend mit Zelle F5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den Prozentsatz der Fertigstellung des Projekts in Spalte G ein, beginnend mit Zelle G5" sqref="H3:H4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Titel des Projekts Geben Sie in dieser Zelle einen neuen Titel ein. Heben Sie einen Zeitraum in H2 hervor. Die Diagrammlegende befindet sich in J2 bis AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Wählen Sie einen hervorzuhebenden Zeitraum in H2 aus. Eine Diagrammlegende befindet sich in J2 bis AI2" sqref="B2:G2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie Aktivitäten in Spalte B ein, beginnend mit Zelle B5_x000a_" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die Dauer des Plans an" sqref="K2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die tatsächliche Dauer an" sqref="Q2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt den Prozentsatz der Fertigstellung des Projekts an" sqref="V2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die tatsächliche Dauer über den Plan hinaus an" sqref="AA2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt den Prozentsatz der Fertigstellung des Projekts über den Plan hinaus an" sqref="AI2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den Startzeitraum des Plans in Spalte C ein, beginnend mit Zelle C5" sqref="D3:D4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie die Dauer in Zeiträumen für den Plan in Spalte D ein, beginnend mit Zelle D5" sqref="E3:E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den tatsächlichen Startzeitraum des Plans in Spalte E ein, beginnend mit Zelle E5" sqref="F3:F4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie die tatsächliche Dauer in Zeiträumen für den Plan in Spalte F ein, beginnend mit Zelle F5" sqref="G3:G4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den Prozentsatz der Fertigstellung des Projekts in Spalte G ein, beginnend mit Zelle G5" sqref="H3:H4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Titel des Projekts Geben Sie in dieser Zelle einen neuen Titel ein. Heben Sie einen Zeitraum in H2 hervor. Die Diagrammlegende befindet sich in J2 bis AI2" sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Wählen Sie einen hervorzuhebenden Zeitraum in H2 aus. Eine Diagrammlegende befindet sich in J2 bis AI2" sqref="B2:G2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie Aktivitäten in Spalte B ein, beginnend mit Zelle B5_x000a_" sqref="C3:C4"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -2208,4 +2271,127 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="27.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="37"/>
+      <c r="B2" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="38">
+        <v>1</v>
+      </c>
+      <c r="E2" s="37"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
+      <c r="B3" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="37">
+        <v>1</v>
+      </c>
+      <c r="E3" s="37"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C5" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="39">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="39">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="39">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added classes for game and screens and a switch to determine game state in setup
</commit_message>
<xml_diff>
--- a/src/documents/Orwb_Gantt.xlsx
+++ b/src/documents/Orwb_Gantt.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>Wählen Sie rechts einen Zeitraum zum Hervorheben aus.  Es folgt eine Legende, die das Diagramm beschreibt.</t>
   </si>
@@ -286,6 +286,30 @@
   </si>
   <si>
     <t>Einarbeitung P5</t>
+  </si>
+  <si>
+    <t>24.01.2019</t>
+  </si>
+  <si>
+    <t>Gravity und Jump implementiert. Code kommentiert</t>
+  </si>
+  <si>
+    <t>Erstellen Gantt Diagramm</t>
+  </si>
+  <si>
+    <t>05.01.2019</t>
+  </si>
+  <si>
+    <t>Beginn Dokumentaion</t>
+  </si>
+  <si>
+    <t>Gespräch mit BMA</t>
+  </si>
+  <si>
+    <t>Führung Journal</t>
+  </si>
+  <si>
+    <t>Dokumentation</t>
   </si>
 </sst>
 </file>
@@ -611,7 +635,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -687,6 +711,15 @@
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -723,14 +756,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1210,10 +1243,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:62" ht="60" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="25"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
@@ -1221,14 +1254,14 @@
       <c r="H1" s="11"/>
     </row>
     <row r="2" spans="2:62" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
       <c r="H2" s="5" t="s">
         <v>31</v>
       </c>
@@ -1236,48 +1269,48 @@
         <v>4</v>
       </c>
       <c r="K2" s="13"/>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="35"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="38"/>
       <c r="Q2" s="19"/>
-      <c r="R2" s="35" t="s">
+      <c r="R2" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
       <c r="V2" s="20"/>
-      <c r="W2" s="26" t="s">
+      <c r="W2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="29"/>
       <c r="AA2" s="18"/>
-      <c r="AB2" s="36" t="s">
+      <c r="AB2" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="36"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="39"/>
       <c r="AI2" s="17"/>
-      <c r="AJ2" s="26" t="s">
+      <c r="AJ2" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="AK2" s="26"/>
-      <c r="AL2" s="26"/>
-      <c r="AM2" s="26"/>
-      <c r="AN2" s="26"/>
-      <c r="AO2" s="26"/>
-      <c r="AP2" s="26"/>
-      <c r="AQ2" s="26"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
+      <c r="AO2" s="29"/>
+      <c r="AP2" s="29"/>
+      <c r="AQ2" s="29"/>
       <c r="AR2" s="15" t="s">
         <v>42</v>
       </c>
@@ -1286,25 +1319,25 @@
       </c>
     </row>
     <row r="3" spans="2:62" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="35" t="s">
         <v>32</v>
       </c>
       <c r="I3" s="14">
@@ -1471,13 +1504,13 @@
       </c>
     </row>
     <row r="4" spans="2:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
       <c r="I4" s="21">
         <v>1</v>
       </c>
@@ -2275,119 +2308,172 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" customWidth="1"/>
+    <col min="2" max="2" width="11.125" style="42" customWidth="1"/>
     <col min="3" max="3" width="23.125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="25" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="25">
+        <v>1</v>
+      </c>
+      <c r="E2" s="25"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
+      <c r="B3" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C3" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D3" s="26">
         <v>1</v>
       </c>
-      <c r="E2" s="37"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37" t="s">
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="26">
+        <v>1</v>
+      </c>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C5" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D5" s="25">
         <v>1</v>
       </c>
-      <c r="E3" s="37"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="E5" s="25"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C6" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="39" t="s">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C7" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D7" s="27">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C8" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D8" s="27">
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="39" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D9" s="27">
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C10" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D10" s="27">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="39" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D11" s="27">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="27">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="27" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>